<commit_message>
Calcul des vecteurs normalisés.
</commit_message>
<xml_diff>
--- a/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
+++ b/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\ProjetsGit\social-dance-jukebox\csharp\Tests\SocialDanceJukebox.Infrastructure.Test\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\Github\social-dance-jukebox\csharp\Tests\SocialDanceJukebox.Infrastructure.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="94">
   <si>
     <t>Nom</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Oldie cover</t>
-  </si>
-  <si>
     <t>Come What May</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
   </si>
   <si>
     <t>Roar</t>
-  </si>
-  <si>
-    <t>Modern cover</t>
   </si>
   <si>
     <t>Être un homme comme vous</t>
@@ -317,7 +311,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,7 +408,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -429,10 +423,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -462,8 +458,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ListeChansons" displayName="ListeChansons" ref="A1:G41" totalsRowShown="0">
   <autoFilter ref="A1:G41"/>
-  <sortState ref="A2:J41">
-    <sortCondition ref="G1:G41"/>
+  <sortState ref="A2:G41">
+    <sortCondition ref="E1:E41"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Nom"/>
@@ -743,9 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -763,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -782,54 +776,54 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>31</v>
+      <c r="A2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>32</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -843,79 +837,79 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
         <v>34</v>
       </c>
-      <c r="C6">
-        <v>36</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
         <v>42</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>28</v>
+      <c r="D8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -923,59 +917,59 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>9</v>
+      <c r="F9" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
       </c>
       <c r="C10">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C11">
-        <v>42</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>12</v>
@@ -983,59 +977,59 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>44</v>
+      <c r="A14" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>38</v>
-      </c>
-      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>28</v>
+      <c r="E14" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>9</v>
@@ -1043,95 +1037,95 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C15">
-        <v>32</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>40</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>33</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
         <v>35</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="8" t="s">
@@ -1142,120 +1136,120 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>92</v>
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
       </c>
       <c r="C21">
-        <v>51</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>12</v>
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
       </c>
       <c r="C22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>83</v>
+      <c r="A23" t="s">
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C23">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>12</v>
+      <c r="E23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C24">
-        <v>41</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>46</v>
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>50</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>90</v>
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>9</v>
@@ -1263,39 +1257,39 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
         <v>36</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27">
-        <v>44</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>16</v>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>9</v>
@@ -1303,75 +1297,75 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C28">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C29">
-        <v>44</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>11</v>
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
       </c>
       <c r="C30">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>12</v>
+      <c r="E30" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" t="s">
-        <v>79</v>
+      <c r="A31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C31">
-        <v>44</v>
-      </c>
-      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -1383,19 +1377,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C32">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>12</v>
@@ -1403,158 +1397,158 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C33">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34">
         <v>42</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34">
+      <c r="D34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37">
         <v>44</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="2">
-        <v>47</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="2">
-        <v>38</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37">
-        <v>42</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>12</v>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2">
-        <v>34</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>12</v>
+      <c r="A38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C39">
-        <v>40</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>44</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="20" t="s">
         <v>28</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -1562,20 +1556,20 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>54</v>
+      <c r="A41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C41" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>55</v>
+      <c r="E41" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Refactoring : injection de tous les composants.
</commit_message>
<xml_diff>
--- a/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
+++ b/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
@@ -66,178 +66,232 @@
     <x:t>Rare</x:t>
   </x:si>
   <x:si>
+    <x:t>Bad Things</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jace Everett</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Standard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Milk And Water</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amos Milburn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Swing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oldie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I'm just a gigolo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Louis Prima</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thank you Very much</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Margaret</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Be My Baby</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bea Miller</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ça ira</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Joyce Jonathan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Français</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hold Me Tight</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Evan Rachel Wood</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oldie Cover</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baby Workout</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jackie Wilson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beyond The Sea</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jeff Lynne</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Come What May</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Etta James</x:t>
+  </x:si>
+  <x:si>
+    <x:t>It's a beautiful Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Michel Bublé</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shake, Rattle And Roll</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hot n Cold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The baseballs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Modern Cover</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feel It Still - Portugal The Man</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Postmodern Jukebox</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Love Me or Leave Me</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Jive Aces</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Don't Stop Me Now </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Queen </x:t>
+  </x:si>
+  <x:si>
+    <x:t>80s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dear Future Husband</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meghan Trainor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What I Like About You</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Romantics</x:t>
+  </x:si>
+  <x:si>
+    <x:t>These Boots are made for walkin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Haley Reinhart</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rockin Robin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Overtones</x:t>
+  </x:si>
+  <x:si>
+    <x:t>T'aint what you do</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Ray Ellington Quartet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reach</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S Club 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pop</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ain't Got No Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Clarence Henry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Johnny B. Goode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cliff Richard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Choo Choo Ch'boogie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Big Bad Voodoo Daddy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>All Shook Up</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Paul McCartney</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coupe de ville</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Si Cranstoun</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Get Over You</x:t>
+  </x:si>
+  <x:si>
+    <x:t>At My Front Door</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The El Dorados</x:t>
+  </x:si>
+  <x:si>
     <x:t>She's the most</x:t>
   </x:si>
   <x:si>
     <x:t>Dick Brave &amp; The Backbeats</x:t>
   </x:si>
   <x:si>
-    <x:t>Oldie Cover</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Come What May</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Etta James</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oldie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Standard</x:t>
-  </x:si>
-  <x:si>
     <x:t>Dance With Me Tonight</x:t>
   </x:si>
   <x:si>
     <x:t>Derek Ryan</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Don't Stop Me Now </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Queen </x:t>
-  </x:si>
-  <x:si>
-    <x:t>80s</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Reach</x:t>
-  </x:si>
-  <x:si>
-    <x:t>S Club 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pop</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Love Me or Leave Me</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Jive Aces</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Swing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Feel It Still - Portugal The Man</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Postmodern Jukebox</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Modern Cover</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Be My Baby</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bea Miller</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Get Over You</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Overtones</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I'm just a gigolo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Louis Prima</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Johnny B. Goode</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cliff Richard</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Coupe de ville</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Si Cranstoun</x:t>
-  </x:si>
-  <x:si>
-    <x:t>All Shook Up</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Paul McCartney</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shake, Rattle And Roll</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Milk And Water</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Amos Milburn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>What I Like About You</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Romantics</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ain't Got No Home</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Clarence Henry</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dear Future Husband</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Meghan Trainor</x:t>
-  </x:si>
-  <x:si>
     <x:t>Tainted Love</x:t>
   </x:si>
   <x:si>
     <x:t>Imelda May</x:t>
   </x:si>
   <x:si>
-    <x:t>Rockin Robin</x:t>
-  </x:si>
-  <x:si>
     <x:t>Let's Get Loud</x:t>
   </x:si>
   <x:si>
-    <x:t>The baseballs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hot n Cold</x:t>
-  </x:si>
-  <x:si>
     <x:t>Only You</x:t>
   </x:si>
   <x:si>
     <x:t>Captain Jack</x:t>
   </x:si>
   <x:si>
-    <x:t>These Boots are made for walkin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Haley Reinhart</x:t>
-  </x:si>
-  <x:si>
-    <x:t>T'aint what you do</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Ray Ellington Quartet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ça ira</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joyce Jonathan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Français</x:t>
+    <x:t>Why Do Fools Fall In Love ?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MMMBop</x:t>
   </x:si>
   <x:si>
     <x:t>Stuck on you</x:t>
@@ -246,61 +300,7 @@
     <x:t>Meiko</x:t>
   </x:si>
   <x:si>
-    <x:t>Baby Workout</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jackie Wilson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>At My Front Door</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The El Dorados</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thank you Very much</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Margaret</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Choo Choo Ch'boogie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Big Bad Voodoo Daddy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bad Things</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jace Everett</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Why Do Fools Fall In Love ?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>It's a beautiful Day</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Michel Bublé</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MMMBop</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Beyond The Sea</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jeff Lynne</x:t>
-  </x:si>
-  <x:si>
     <x:t>Roar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hold Me Tight</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Evan Rachel Wood</x:t>
   </x:si>
   <x:si>
     <x:t>Être un homme comme vous</x:t>
@@ -416,26 +416,26 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="20">
+  <x:cellXfs count="22">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -443,13 +443,13 @@
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -458,7 +458,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -466,11 +466,19 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -583,118 +591,118 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>32</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>33</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>36</c:v>
-                </c:pt>
                 <c:pt idx="35">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>34</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>51</c:v>
@@ -713,11 +721,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="549702648"/>
-        <c:axId val="549705000"/>
+        <c:axId val="565557640"/>
+        <c:axId val="565561168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="549702648"/>
+        <c:axId val="565557640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +767,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549705000"/>
+        <c:crossAx val="565561168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -767,7 +775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="549705000"/>
+        <c:axId val="565561168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +826,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549702648"/>
+        <c:crossAx val="565557640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,7 +1805,7 @@
     </x:row>
     <x:row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="n">
-        <x:v>31</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>13</x:v>
@@ -1806,24 +1814,24 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F3" s="16" t="s">
+      <x:c r="F3" s="14" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G3" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G3" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>16</x:v>
@@ -1832,24 +1840,24 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F4" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G4" s="18" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G4" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>20</x:v>
@@ -1858,342 +1866,342 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F5" s="16" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F5" s="17" t="s">
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G5" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B6" s="10" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C6" s="11" t="s">
+      <x:c r="C6" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F6" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G6" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F6" s="18" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G6" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A7" s="1" t="n">
-        <x:v>23</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
       <x:c r="D7" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F7" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G7" s="18" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G7" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="n">
-        <x:v>16</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="n">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F8" s="19" t="s">
+      <x:c r="F8" s="18" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G8" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G8" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="n">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F9" s="18" t="s">
+      <x:c r="G9" s="15" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="n">
         <x:v>33</x:v>
-      </x:c>
-      <x:c r="G9" s="18" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="n">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="n">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="n">
-        <x:v>33</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F10" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G10" s="18" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G10" s="15" t="s">
+        <x:v>12</x:v>
+      </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="n">
-        <x:v>29</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F11" s="17" t="s">
-        <x:v>18</x:v>
+      <x:c r="F11" s="19" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G11" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="n">
-        <x:v>4</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F12" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G12" s="15" t="s">
-        <x:v>12</x:v>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G12" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="n">
-        <x:v>25</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D13" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F13" s="16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G13" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F13" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G13" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A14" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
-        <x:v>43</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="D14" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E14" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F14" s="16" t="s">
+      <x:c r="F14" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G14" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G14" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D15" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F15" s="16" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G15" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G15" s="18" t="s">
-        <x:v>19</x:v>
-      </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A16" s="1" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F16" s="16" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G16" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="n">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="n">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F16" s="16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G16" s="18" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H16" s="0" t="n">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A17" s="1" t="n">
-        <x:v>3</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
       <x:c r="D17" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F17" s="17" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="G17" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F17" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G17" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="n">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B18" s="20" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C18" s="20" t="s">
         <x:v>50</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>51</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
         <x:v>40</x:v>
@@ -2201,19 +2209,19 @@
       <x:c r="E18" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F18" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G18" s="15" t="s">
-        <x:v>12</x:v>
+      <x:c r="F18" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G18" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A19" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
         <x:v>52</x:v>
@@ -2222,24 +2230,24 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F19" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G19" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F19" s="14" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G19" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A20" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
         <x:v>54</x:v>
@@ -2253,19 +2261,19 @@
       <x:c r="E20" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F20" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G20" s="18" t="s">
+      <x:c r="F20" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G20" s="15" t="s">
+        <x:v>12</x:v>
+      </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A21" s="1" t="n">
-        <x:v>33</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
         <x:v>56</x:v>
@@ -2274,19 +2282,19 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="D21" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F21" s="16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G21" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F21" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G21" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2297,7 +2305,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
         <x:v>41</x:v>
@@ -2305,222 +2313,222 @@
       <x:c r="E22" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F22" s="16" t="s">
-        <x:v>15</x:v>
+      <x:c r="F22" s="19" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G22" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A23" s="1" t="n">
-        <x:v>34</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D23" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F23" s="16" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F23" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G23" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G23" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A24" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D24" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F24" s="18" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G24" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="F24" s="14" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G24" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A25" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D25" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F25" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G25" s="18" t="s">
+      <x:c r="F25" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G25" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A26" s="1" t="n">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D26" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F26" s="16" t="s">
+      <x:c r="F26" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G26" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G26" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A27" s="1" t="n">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D27" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F27" s="16" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F27" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G27" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G27" s="18" t="s">
-        <x:v>19</x:v>
-      </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A28" s="1" t="n">
-        <x:v>7</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D28" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="F28" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G28" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F28" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G28" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A29" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D29" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F29" s="14" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F29" s="19" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G29" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A30" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D30" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F30" s="17" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G30" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,10 +2536,10 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D31" s="0" t="n">
         <x:v>44</x:v>
@@ -2540,247 +2548,247 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F31" s="17" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G31" s="18" t="s">
         <x:v>19</x:v>
       </x:c>
+      <x:c r="G31" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A32" s="1" t="n">
-        <x:v>5</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D32" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F32" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G32" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F32" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G32" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A33" s="1" t="n">
-        <x:v>26</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D33" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F33" s="16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G33" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F33" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G33" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A34" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D34" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F34" s="14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G34" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F34" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G34" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A35" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D35" s="0" t="n">
-        <x:v>47</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F35" s="16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G35" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F35" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G35" s="15" t="s">
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A36" s="1" t="n">
-        <x:v>12</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="D36" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E36" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F36" s="16" t="s">
+      <x:c r="F36" s="14" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G36" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G36" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A37" s="1" t="n">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F37" s="19" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G37" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H37" s="0" t="n">
         <x:v>32</x:v>
-      </x:c>
-      <x:c r="D37" s="0" t="n">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E37" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F37" s="18" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G37" s="15" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="H37" s="0" t="n">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A38" s="1" t="n">
-        <x:v>10</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D38" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E38" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F38" s="16" t="s">
-        <x:v>15</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G38" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A39" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
         <x:v>89</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D39" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F39" s="18" t="s">
-        <x:v>33</x:v>
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="F39" s="14" t="s">
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G39" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A40" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D40" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E40" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F40" s="19" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F40" s="21" t="s">
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G40" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2799,11 +2807,11 @@
       <x:c r="E41" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="F41" s="18" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G41" s="18" t="s">
-        <x:v>19</x:v>
+      <x:c r="F41" s="16" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G41" s="16" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
         <x:v>40</x:v>

</xml_diff>

<commit_message>
Ajout d'une distance binaire.
</commit_message>
<xml_diff>
--- a/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
+++ b/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
@@ -435,20 +435,20 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="22">
+  <x:cellXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -471,10 +471,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -721,11 +717,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="565557640"/>
-        <c:axId val="565561168"/>
+        <c:axId val="452809888"/>
+        <c:axId val="564932040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565557640"/>
+        <c:axId val="452809888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +763,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565561168"/>
+        <c:crossAx val="564932040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -775,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565561168"/>
+        <c:axId val="564932040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +822,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565557640"/>
+        <c:crossAx val="452809888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1852,7 +1848,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1878,7 +1874,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1930,7 +1926,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1956,7 +1952,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1982,7 +1978,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2008,7 +2004,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2034,7 +2030,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2060,7 +2056,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2086,7 +2082,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2138,7 +2134,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2164,7 +2160,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2190,17 +2186,17 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="n">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B18" s="20" t="s">
+      <x:c r="B18" s="12" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C18" s="20" t="s">
+      <x:c r="C18" s="12" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
@@ -2216,7 +2212,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,7 +2238,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,7 +2264,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2294,7 +2290,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2320,7 +2316,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2346,7 +2342,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2372,7 +2368,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2398,7 +2394,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2424,7 +2420,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2450,7 +2446,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2476,7 +2472,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2502,7 +2498,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,7 +2524,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2554,7 +2550,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2580,7 +2576,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,7 +2602,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2632,7 +2628,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,7 +2654,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2684,7 +2680,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2710,7 +2706,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2736,7 +2732,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2762,7 +2758,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2781,14 +2777,14 @@
       <x:c r="E40" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F40" s="21" t="s">
+      <x:c r="F40" s="20" t="s">
         <x:v>44</x:v>
       </x:c>
       <x:c r="G40" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout sélecteur meilleur candidat.
</commit_message>
<xml_diff>
--- a/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
+++ b/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
@@ -435,13 +435,11 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="22">
+  <x:cellXfs count="20">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -450,7 +448,7 @@
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -718,11 +716,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="565586256"/>
-        <c:axId val="565585864"/>
+        <c:axId val="593634480"/>
+        <c:axId val="593627032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565586256"/>
+        <c:axId val="593634480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,7 +762,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565585864"/>
+        <c:crossAx val="593627032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -772,7 +770,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565585864"/>
+        <c:axId val="593627032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +821,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565586256"/>
+        <c:crossAx val="593634480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1790,10 +1788,10 @@
       <x:c r="E2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F2" s="15" t="s">
+      <x:c r="F2" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G2" s="16" t="s">
+      <x:c r="G2" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
@@ -1816,14 +1814,14 @@
       <x:c r="E3" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F3" s="15" t="s">
+      <x:c r="F3" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G3" s="17" t="s">
+      <x:c r="G3" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,14 +1840,14 @@
       <x:c r="E4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F4" s="18" t="s">
+      <x:c r="F4" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G4" s="17" t="s">
+      <x:c r="G4" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,14 +1866,14 @@
       <x:c r="E5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F5" s="18" t="s">
+      <x:c r="F5" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G5" s="16" t="s">
+      <x:c r="G5" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,14 +1892,14 @@
       <x:c r="E6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F6" s="19" t="s">
+      <x:c r="F6" s="17" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G6" s="17" t="s">
+      <x:c r="G6" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1920,14 +1918,14 @@
       <x:c r="E7" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F7" s="18" t="s">
+      <x:c r="F7" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G7" s="17" t="s">
+      <x:c r="G7" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1946,14 +1944,14 @@
       <x:c r="E8" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="F8" s="19" t="s">
+      <x:c r="F8" s="17" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G8" s="17" t="s">
+      <x:c r="G8" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1972,10 +1970,10 @@
       <x:c r="E9" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F9" s="20" t="s">
+      <x:c r="F9" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G9" s="16" t="s">
+      <x:c r="G9" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
@@ -1998,14 +1996,14 @@
       <x:c r="E10" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F10" s="18" t="s">
+      <x:c r="F10" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G10" s="16" t="s">
+      <x:c r="G10" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2024,14 +2022,14 @@
       <x:c r="E11" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F11" s="20" t="s">
+      <x:c r="F11" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G11" s="16" t="s">
+      <x:c r="G11" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2050,14 +2048,14 @@
       <x:c r="E12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F12" s="18" t="s">
+      <x:c r="F12" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G12" s="17" t="s">
+      <x:c r="G12" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2076,14 +2074,14 @@
       <x:c r="E13" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F13" s="20" t="s">
+      <x:c r="F13" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G13" s="16" t="s">
+      <x:c r="G13" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2102,14 +2100,14 @@
       <x:c r="E14" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F14" s="20" t="s">
+      <x:c r="F14" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G14" s="17" t="s">
+      <x:c r="G14" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2128,14 +2126,14 @@
       <x:c r="E15" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F15" s="17" t="s">
+      <x:c r="F15" s="15" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G15" s="17" t="s">
+      <x:c r="G15" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2154,14 +2152,14 @@
       <x:c r="E16" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F16" s="17" t="s">
+      <x:c r="F16" s="15" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G16" s="17" t="s">
+      <x:c r="G16" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2180,24 +2178,24 @@
       <x:c r="E17" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F17" s="20" t="s">
+      <x:c r="F17" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G17" s="16" t="s">
+      <x:c r="G17" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="n">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B18" s="6" t="s">
+      <x:c r="B18" s="4" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C18" s="6" t="s">
+      <x:c r="C18" s="4" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
@@ -2209,11 +2207,11 @@
       <x:c r="F18" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="G18" s="17" t="s">
+      <x:c r="G18" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2232,14 +2230,14 @@
       <x:c r="E19" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F19" s="15" t="s">
+      <x:c r="F19" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G19" s="17" t="s">
+      <x:c r="G19" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2258,14 +2256,14 @@
       <x:c r="E20" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F20" s="18" t="s">
+      <x:c r="F20" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G20" s="16" t="s">
+      <x:c r="G20" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2284,14 +2282,14 @@
       <x:c r="E21" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F21" s="20" t="s">
+      <x:c r="F21" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G21" s="16" t="s">
+      <x:c r="G21" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2310,14 +2308,14 @@
       <x:c r="E22" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F22" s="20" t="s">
+      <x:c r="F22" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G22" s="16" t="s">
+      <x:c r="G22" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2336,14 +2334,14 @@
       <x:c r="E23" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F23" s="20" t="s">
+      <x:c r="F23" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G23" s="17" t="s">
+      <x:c r="G23" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2362,14 +2360,14 @@
       <x:c r="E24" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="F24" s="15" t="s">
+      <x:c r="F24" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G24" s="17" t="s">
+      <x:c r="G24" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2388,14 +2386,14 @@
       <x:c r="E25" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F25" s="18" t="s">
+      <x:c r="F25" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G25" s="17" t="s">
+      <x:c r="G25" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2414,14 +2412,14 @@
       <x:c r="E26" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F26" s="20" t="s">
+      <x:c r="F26" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G26" s="17" t="s">
+      <x:c r="G26" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2440,14 +2438,14 @@
       <x:c r="E27" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F27" s="20" t="s">
+      <x:c r="F27" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G27" s="17" t="s">
+      <x:c r="G27" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2466,14 +2464,14 @@
       <x:c r="E28" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F28" s="20" t="s">
+      <x:c r="F28" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G28" s="17" t="s">
+      <x:c r="G28" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2492,14 +2490,14 @@
       <x:c r="E29" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F29" s="20" t="s">
+      <x:c r="F29" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G29" s="16" t="s">
+      <x:c r="G29" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2518,14 +2516,14 @@
       <x:c r="E30" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F30" s="18" t="s">
+      <x:c r="F30" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G30" s="16" t="s">
+      <x:c r="G30" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2544,14 +2542,14 @@
       <x:c r="E31" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F31" s="18" t="s">
+      <x:c r="F31" s="16" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G31" s="17" t="s">
+      <x:c r="G31" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2570,14 +2568,14 @@
       <x:c r="E32" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F32" s="20" t="s">
+      <x:c r="F32" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G32" s="16" t="s">
+      <x:c r="G32" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2596,14 +2594,14 @@
       <x:c r="E33" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F33" s="20" t="s">
+      <x:c r="F33" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G33" s="16" t="s">
+      <x:c r="G33" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2622,14 +2620,14 @@
       <x:c r="E34" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F34" s="20" t="s">
+      <x:c r="F34" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G34" s="17" t="s">
+      <x:c r="G34" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2648,14 +2646,14 @@
       <x:c r="E35" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F35" s="20" t="s">
+      <x:c r="F35" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G35" s="16" t="s">
+      <x:c r="G35" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2674,14 +2672,14 @@
       <x:c r="E36" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F36" s="15" t="s">
+      <x:c r="F36" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G36" s="17" t="s">
+      <x:c r="G36" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2700,14 +2698,14 @@
       <x:c r="E37" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F37" s="20" t="s">
+      <x:c r="F37" s="18" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G37" s="17" t="s">
+      <x:c r="G37" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2726,14 +2724,14 @@
       <x:c r="E38" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F38" s="17" t="s">
+      <x:c r="F38" s="15" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G38" s="16" t="s">
+      <x:c r="G38" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2752,14 +2750,14 @@
       <x:c r="E39" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="F39" s="15" t="s">
+      <x:c r="F39" s="13" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G39" s="16" t="s">
+      <x:c r="G39" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2778,14 +2776,14 @@
       <x:c r="E40" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F40" s="21" t="s">
+      <x:c r="F40" s="19" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G40" s="16" t="s">
+      <x:c r="G40" s="14" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2804,14 +2802,14 @@
       <x:c r="E41" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="F41" s="17" t="s">
+      <x:c r="F41" s="15" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G41" s="17" t="s">
+      <x:c r="G41" s="15" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Ajout sélecteur vecteur avec le plus de voisins proches.
</commit_message>
<xml_diff>
--- a/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
+++ b/csharp/Tests/SocialDanceJukebox.Infrastructure.Test/Resources/DataChansons.xlsx
@@ -435,20 +435,21 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="20">
+  <x:cellXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -716,11 +717,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="593634480"/>
-        <c:axId val="593627032"/>
+        <c:axId val="565431112"/>
+        <c:axId val="565431896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="593634480"/>
+        <c:axId val="565431112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +763,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593627032"/>
+        <c:crossAx val="565431896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -770,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="593627032"/>
+        <c:axId val="565431896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +822,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593634480"/>
+        <c:crossAx val="565431112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,10 +1789,10 @@
       <x:c r="E2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F2" s="13" t="s">
+      <x:c r="F2" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G2" s="14" t="s">
+      <x:c r="G2" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H2" s="0" t="n">
@@ -1814,14 +1815,14 @@
       <x:c r="E3" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F3" s="13" t="s">
+      <x:c r="F3" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G3" s="15" t="s">
+      <x:c r="G3" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1840,14 +1841,14 @@
       <x:c r="E4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F4" s="16" t="s">
+      <x:c r="F4" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G4" s="15" t="s">
+      <x:c r="G4" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H4" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1866,14 +1867,14 @@
       <x:c r="E5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F5" s="16" t="s">
+      <x:c r="F5" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G5" s="14" t="s">
+      <x:c r="G5" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1892,14 +1893,14 @@
       <x:c r="E6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F6" s="17" t="s">
+      <x:c r="F6" s="18" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G6" s="15" t="s">
+      <x:c r="G6" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H6" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,14 +1919,14 @@
       <x:c r="E7" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F7" s="16" t="s">
+      <x:c r="F7" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G7" s="15" t="s">
+      <x:c r="G7" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H7" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1944,14 +1945,14 @@
       <x:c r="E8" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="F8" s="17" t="s">
+      <x:c r="F8" s="18" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G8" s="15" t="s">
+      <x:c r="G8" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H8" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1970,14 +1971,14 @@
       <x:c r="E9" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F9" s="18" t="s">
+      <x:c r="F9" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G9" s="14" t="s">
+      <x:c r="G9" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H9" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1996,14 +1997,14 @@
       <x:c r="E10" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F10" s="16" t="s">
+      <x:c r="F10" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G10" s="14" t="s">
+      <x:c r="G10" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H10" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2022,14 +2023,14 @@
       <x:c r="E11" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F11" s="18" t="s">
+      <x:c r="F11" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G11" s="14" t="s">
+      <x:c r="G11" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H11" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2048,14 +2049,14 @@
       <x:c r="E12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F12" s="16" t="s">
+      <x:c r="F12" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G12" s="15" t="s">
+      <x:c r="G12" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H12" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2074,14 +2075,14 @@
       <x:c r="E13" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F13" s="18" t="s">
+      <x:c r="F13" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G13" s="14" t="s">
+      <x:c r="G13" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H13" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2100,14 +2101,14 @@
       <x:c r="E14" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F14" s="18" t="s">
+      <x:c r="F14" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G14" s="15" t="s">
+      <x:c r="G14" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H14" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2126,14 +2127,14 @@
       <x:c r="E15" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F15" s="15" t="s">
+      <x:c r="F15" s="16" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G15" s="15" t="s">
+      <x:c r="G15" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2152,14 +2153,14 @@
       <x:c r="E16" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F16" s="15" t="s">
+      <x:c r="F16" s="16" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G16" s="15" t="s">
+      <x:c r="G16" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H16" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2178,14 +2179,14 @@
       <x:c r="E17" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F17" s="18" t="s">
+      <x:c r="F17" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G17" s="14" t="s">
+      <x:c r="G17" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H17" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2207,11 +2208,11 @@
       <x:c r="F18" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="G18" s="15" t="s">
+      <x:c r="G18" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H18" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2230,14 +2231,14 @@
       <x:c r="E19" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F19" s="13" t="s">
+      <x:c r="F19" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G19" s="15" t="s">
+      <x:c r="G19" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H19" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2256,14 +2257,14 @@
       <x:c r="E20" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F20" s="16" t="s">
+      <x:c r="F20" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G20" s="14" t="s">
+      <x:c r="G20" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H20" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2282,14 +2283,14 @@
       <x:c r="E21" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F21" s="18" t="s">
+      <x:c r="F21" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G21" s="14" t="s">
+      <x:c r="G21" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H21" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2308,14 +2309,14 @@
       <x:c r="E22" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F22" s="18" t="s">
+      <x:c r="F22" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G22" s="14" t="s">
+      <x:c r="G22" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H22" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2334,14 +2335,14 @@
       <x:c r="E23" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F23" s="18" t="s">
+      <x:c r="F23" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G23" s="15" t="s">
+      <x:c r="G23" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H23" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2360,14 +2361,14 @@
       <x:c r="E24" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="F24" s="13" t="s">
+      <x:c r="F24" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G24" s="15" t="s">
+      <x:c r="G24" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H24" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2386,14 +2387,14 @@
       <x:c r="E25" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F25" s="16" t="s">
+      <x:c r="F25" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G25" s="15" t="s">
+      <x:c r="G25" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H25" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2412,14 +2413,14 @@
       <x:c r="E26" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F26" s="18" t="s">
+      <x:c r="F26" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G26" s="15" t="s">
+      <x:c r="G26" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H26" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2438,14 +2439,14 @@
       <x:c r="E27" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F27" s="18" t="s">
+      <x:c r="F27" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G27" s="15" t="s">
+      <x:c r="G27" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H27" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2464,14 +2465,14 @@
       <x:c r="E28" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F28" s="18" t="s">
+      <x:c r="F28" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G28" s="15" t="s">
+      <x:c r="G28" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H28" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2490,14 +2491,14 @@
       <x:c r="E29" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F29" s="18" t="s">
+      <x:c r="F29" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G29" s="14" t="s">
+      <x:c r="G29" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H29" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2516,14 +2517,14 @@
       <x:c r="E30" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F30" s="16" t="s">
+      <x:c r="F30" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G30" s="14" t="s">
+      <x:c r="G30" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H30" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,14 +2543,14 @@
       <x:c r="E31" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F31" s="16" t="s">
+      <x:c r="F31" s="17" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G31" s="15" t="s">
+      <x:c r="G31" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H31" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2568,14 +2569,14 @@
       <x:c r="E32" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F32" s="18" t="s">
+      <x:c r="F32" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G32" s="14" t="s">
+      <x:c r="G32" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H32" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2594,14 +2595,14 @@
       <x:c r="E33" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F33" s="18" t="s">
+      <x:c r="F33" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G33" s="14" t="s">
+      <x:c r="G33" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H33" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2620,14 +2621,14 @@
       <x:c r="E34" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F34" s="18" t="s">
+      <x:c r="F34" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G34" s="15" t="s">
+      <x:c r="G34" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H34" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2646,14 +2647,14 @@
       <x:c r="E35" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F35" s="18" t="s">
+      <x:c r="F35" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G35" s="14" t="s">
+      <x:c r="G35" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H35" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2672,14 +2673,14 @@
       <x:c r="E36" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F36" s="13" t="s">
+      <x:c r="F36" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G36" s="15" t="s">
+      <x:c r="G36" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H36" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2698,14 +2699,14 @@
       <x:c r="E37" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F37" s="18" t="s">
+      <x:c r="F37" s="19" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G37" s="15" t="s">
+      <x:c r="G37" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H37" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2724,14 +2725,14 @@
       <x:c r="E38" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F38" s="15" t="s">
+      <x:c r="F38" s="16" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G38" s="14" t="s">
+      <x:c r="G38" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H38" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2750,14 +2751,14 @@
       <x:c r="E39" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="F39" s="13" t="s">
+      <x:c r="F39" s="14" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G39" s="14" t="s">
+      <x:c r="G39" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H39" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2776,14 +2777,14 @@
       <x:c r="E40" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F40" s="19" t="s">
+      <x:c r="F40" s="20" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G40" s="14" t="s">
+      <x:c r="G40" s="15" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="H40" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2802,14 +2803,14 @@
       <x:c r="E41" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="F41" s="15" t="s">
+      <x:c r="F41" s="16" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G41" s="15" t="s">
+      <x:c r="G41" s="16" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>